<commit_message>
Extended dialog converion tool, additional validation added. New intro. Some fixes in dialogs
</commit_message>
<xml_diff>
--- a/doc/dialog sources/������.xlsx
+++ b/doc/dialog sources/������.xlsx
@@ -1082,10 +1082,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1346,7 +1346,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>31</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>14</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>33</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>15</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>34</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>35</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>61</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>36</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>16</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>38</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>19</v>
       </c>
@@ -1434,18 +1434,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>42</v>
       </c>
       <c r="C44">
         <v>-1</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>17</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>41</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>18</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>44</v>
       </c>

</xml_diff>